<commit_message>
Replaced Clustering+Classification by Clustering+MetricLearning
</commit_message>
<xml_diff>
--- a/featuresinputexcel.xlsx
+++ b/featuresinputexcel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanbraun/PycharmProjects/WebServices/BestPracticeSharingApp/BestPracticeSharing/MicroserviceBackend/DataImportService/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stefanbraun/PycharmProjects/BestPracticeSharing-Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E187380E-63EF-F246-9ABB-1C1416F472A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96BED88-77BB-DC47-B576-68D85B48BAA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="20600" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C751"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -412,10 +412,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.49426096724941138</v>
+        <v>0.4</v>
       </c>
       <c r="B2">
-        <v>1.4510669654101751</v>
+        <v>2.5</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -423,10 +423,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>-1.4280809932351519</v>
+        <v>0.43</v>
       </c>
       <c r="B3">
-        <v>-0.83706376669002469</v>
+        <v>3.23</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -434,10 +434,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0.33855918238435578</v>
+        <v>2.13</v>
       </c>
       <c r="B4">
-        <v>1.0387587093943791</v>
+        <v>0.86</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -445,10 +445,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>0.1190010137807008</v>
+        <v>2.1</v>
       </c>
       <c r="B5">
-        <v>-1.053975533363686</v>
+        <v>3.23</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -456,10 +456,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.122424604448669</v>
+        <v>0.43</v>
       </c>
       <c r="B6">
-        <v>1.7749365443638381</v>
+        <v>1.5</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -467,10 +467,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-1.261569897067039</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B7">
-        <v>0.27188135429934829</v>
+        <v>1.53</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>-1.3015477462579139</v>
+        <v>2.1</v>
       </c>
       <c r="B8">
-        <v>-0.76206202514798282</v>
+        <v>1.8</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -489,10 +489,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0.58569865152093781</v>
+        <v>1.8</v>
       </c>
       <c r="B9">
-        <v>-0.33910462815669962</v>
+        <v>1.8</v>
       </c>
       <c r="C9">
         <v>2</v>

</xml_diff>